<commit_message>
Get daily reddit data: Tue Oct  1 08:11:03 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_06.xlsx
+++ b/data/collected_data/2024_10_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C479"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3032 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1ftiu35</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>New here! So here's some sets I've had over the years</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftiu35</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1ftirus</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m in love with my nail art! Who else loves creative designs </t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3bx36ypnp3sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1ftinwi</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Gel Polish lifts from the tip??!!</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ftinwi/gel_polish_lifts_from_the_tip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1fthh8k</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So obsessed </t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fthh8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1fthaap</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Poison Ivy Nails</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fthaap</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1ftgpf5</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>How long do you guys wait to get infill? I hate the gaps that show. I’ve never had an infill done. Do the nails look like before after getting an infill?</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/420b0ny7z2sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1ftg9eq</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Tortoise French tips!</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftg9eq</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1ftdymv</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Should I just pull the plug? 😭</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftdymv</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1ftevd1</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>How to get glue off my nails?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25yaefetf2sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1fte9gu</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Ingrown removal at salon?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fte9gu/ingrown_removal_at_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1ftcr0z</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Is it worth it to book with a random or same nail tech?</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ftcr0z/is_it_worth_it_to_book_with_a_random_or_same_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1ftejy2</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Ghosties</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04bvjb9oc2sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1fteis6</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed with my new nails! </t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fteis6</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1ftehk5</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>My first try at fairy nails 🧚‍♀️</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftehk5</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1ftea0h</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>The best money spent this month 💅🏻💞💎</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0kpw4cz92sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1fte6eh</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>I’m really loving my Halloween set this year~ 🖤❤️😈💅🏾</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vnhb925092sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1fte0ur</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Ready for spring 🏵️</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgdsy56772sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1ftddzl</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Music Inspired Nails: Spiritbox "Soft Spine"</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftddzl</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1ftc5d3</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>what i got vs. inspo pic!</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftc5d3</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1ftd9sy</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aztec calendar nails </t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ftd9sy/aztec_calendar_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1ftcd95</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Ghosties</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6bf4t8es1sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1ftbgkx</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Ready for fall weather</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ftbgkx/ready_for_fall_weather/</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1ftbdrd</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Heat Sensitive Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftbdrd</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1ftbmd7</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky Season Vibes Activated </t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftbmd7</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1fta73t</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I need some help with my press on nail issues </t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fta73t/i_need_some_help_with_my_press_on_nail_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1ft7s0c</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Inspo nails from this group!</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft7s0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1ft9hmj</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Butterfly 🦋 </t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft9hmj</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1ft6soc</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>2nd time doing gelx!</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yqkiaqmmi0sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1ft9fvl</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It's fall y'all </t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3sphnu631sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1ft9frc</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>One Piece Wanted Posters 🏴‍☠️</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft9frc</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1ft70sv</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>I hate how they look from underneath…</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft70sv</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1ft9fn4</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Would you paint your toenails blue to match too?</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/akmyiov431sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1ft9a2w</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>My two favorite aesthetics in one set. Spooky and girly</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1ab3nkw11sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1ft8fc0</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Tomorrow is Oct (aka the most wonderful time of the year)</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w74zpg72v0sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1ft7z8g</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First fall ish set of the year </t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2z25a9jr0sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1ft7dyh</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gilded  garden ✨  </t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w9vmzrgzm0sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1ft6u2y</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>I miss them being big, the process of letting them grow is very slow</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft6u2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1ft6r41</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best brand of sturdy press-on nails? </t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ft6r41/best_brand_of_sturdy_presson_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1ft6ln5</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Anyone know why this might be happening/how to fix?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft6ln5</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1ft6bg8</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>the prettiest nails i’ve had :D</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft6bg8</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1ft678b</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t xml:space="preserve">October nails </t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/znmdzyvae0sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1ft5dau</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>opinions on these nails i did myself?</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jddok8zc80sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1ft5lpf</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>My tech commented on my dry hands :( Lotion recs?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ft5lpf/my_tech_commented_on_my_dry_hands_lotion_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1ft584c</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>First spooky set of the season. Obsessed with how they came out 👻🎃</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft584c</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1ft511c</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I tried😅anyone recommend  good brushes for detailed art on nails </t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xi2je9os50sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1ft441x</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>How do i get builder gel to stop lifting at the free edge?</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ft441x/how_do_i_get_builder_gel_to_stop_lifting_at_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1ft3ork</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft3ork</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1ft3jnc</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>In love with my new set</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/orc3nplxuzrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1ft3e1m</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Starting Nail School</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ft3e1m/starting_nail_school/</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1ft3b2n</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spicy 🌶️ </t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4ai2q28tzrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1ft39d5</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Queen of grape nails 🍇 also starring a very derpy boy </t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft39d5</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1ft2yt9</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love doing extra nails but I’ll always gravitate back to a classic red </t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ce55h1wrqzrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1ft2u86</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>pink scales 🐢</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft2u86</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1ft2g89</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Autumn 🍂 nails inspo</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ft2g89/autumn_nails_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1ft2cdc</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Why does my structured manicure keep lifting</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ft2cdc/why_does_my_structured_manicure_keep_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1ft2fp7</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Matte top coat on press ons</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft2fp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1ft1yn8</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Glow in the dark shroom gel set done by me 👽☄️🌈🍄‍🟫🍄💅🏾</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft1yn8</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1ft1xee</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>👻🕸️🕷️</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft1xee</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1ft1weh</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>what are your thoughts about press ons</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/92i7wbpdizrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1ft1w2g</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Cat eye with Chrome 💅💗</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft1w2g</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1ft1e74</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I want to start doing nails at home. Tips? </t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ft1e74/i_want_to_start_doing_nails_at_home_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1ft17ol</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel overlay with extensions </t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ft17ol/gel_overlay_with_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1ft13o4</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Sweetiepie nails</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft13o4</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1ft0xqu</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Tried something extra colorful 💜💫</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft0xqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1ft0d4h</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>jelly mermaid nails 🧜‍♀️💅🪼</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2y9uuiv7zrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1fszwq9</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>🌹</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y4veublk4zrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1fszobb</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>My nude nails Im in love with</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w9j9z7qw2zrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1fszhes</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Matte autumn nails 🍂🟤</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fszhes</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1fszeuh</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fszeuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1fsz36t</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Newbie questions for engagement photos! </t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fsz36t/newbie_questions_for_engagement_photos/</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1fsxrjb</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>✨🔮✨</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oiwdp786pyrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1fsygz9</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Spoopy inspired nails</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fsygz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1fsyxzi</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Cracked UV Gel Nail</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fsyxzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1fsndyf</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Acrylic removal</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fsndyf/acrylic_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1fsqfmu</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>did i apply my press ons okay? it's my first time</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fsqfmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1fsxzdg</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>SOS- What am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fsxzdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1fsywg9</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>so proud of my growth</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fsywg9</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1fsytdv</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>UK! Desperate to find this discontinued Boots cuticle oil - or an alternative [see description]</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4dxxzctwyrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1fsys86</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can’t go wrong with a French tip 💅🏼 </t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z9h56oflwyrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1fsy9wq</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Just got my nails done! All spooky and glittery for halloween :)</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbauf0klmyrd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1fsy9mu</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t xml:space="preserve">little cuties </t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/253ptl4vsyrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1fsy3z4</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>I kinda like this color</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4llyjlnryrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1fsxeua</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Just natural nails</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qliig4fjmyrd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1fswjxq</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Where do y’all buy your nail art stickers?</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fswjxq/where_do_yall_buy_your_nail_art_stickers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1fsw6up</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I just got my nails done by an at home tech for the first time thoughts? I love them </t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fsw6up</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1fsvc4m</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>August set</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fsvc4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1fsuioj</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Nail set I did for an upcoming concert ⛓️🖇️🥀</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fsuioj</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1fsu9x6</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>If you use builder gel to grow out your natural nails, do you also use top coat?</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fsu9x6/if_you_use_builder_gel_to_grow_out_your_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1fstt1s</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Customer's request for such a design </t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xh0zxg96sxrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1fstdtx</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Nail Shape?</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqdkxv82oxrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1fsta3v</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Work Gloves for Long Nails?</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8i9qm9mymxrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1fssz5c</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>it's finally my time (I love dark nails)</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fssz5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1fssubk</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Nail of the month</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fssubk</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1fss50l</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Luminous green with orange are my happy nail colors. Did a splash instead of ombre this time. What do we think?</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fss50l</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1fsrjxg</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>In love!! so happy with how these turned out</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5i4ls682xrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1fsrbmf</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Loving my holiday nails</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1za3bob1zwrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1fsqtt4</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>New nails in prep for Halloween!!</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h59czaq0swrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1fsqja8</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Do these look like press ons or can they pass as not press ons ❓</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lrrb7rrtnwrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1fthfr2</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Had my husband pick my last manicure before I cut my nails down</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fthfr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1fthalg</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Am I being overly critical of my manicure?</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7tk0xr9163sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1fth5rj</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Get the Perfect At-Home Manicure with Modelones’ Pleascent Nail Care Routine for 10-20% Off on Amazon Prime Day!</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fth5rj/get_the_perfect_athome_manicure_with_modelones/</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1ftew5d</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>orange equivalent of sour apple rings?</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ftew5d/orange_equivalent_of_sour_apple_rings/</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1ftekp6</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Joni’s response Drunk Fairy Polish</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftekp6</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1fteix7</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>My short fall nails</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29rnmcqdc2sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1ftdsfl</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First starrily haul. Their packaging is adorable </t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mp4qrmma52sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1ftdqpn</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Toxic sludge yay!</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftdqpn</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1ftcnj2</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did it different for today </t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/96j94bkwu1sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1ftchu3</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>ILNP Hallucinate ❤️✨</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5wviz2it1sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1ftbsvc</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>First post! I had to show these colors off, I really like how they look together 😄</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftbsvc</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1ftayro</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Mermaid Bait</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftayro</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1ft9io5</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Can't adequately capture how gorgeous this is ✨️</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft9io5</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1ft99k7</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>So sad</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft99k7</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1ft93ly</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP Candlelight </t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ipus0cmg01sd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1ft8d12</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Man of La Mancha</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft89ov</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1ft82rk</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Slowly trying out more nail art</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft82rk</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1ft80hv</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>monarch really did that tho</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft80hv</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1ft7spf</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>One Chip in Manicure</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ix16gc6q0sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1ft7fxu</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Go Home</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft7fxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1ft5vjf</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>pretend nail polish for my pre-k students 🥰💅</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhh94opwb0sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1ft5mot</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Warm toned red color match: Orly vs Jinsoon</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft5mot</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1ft50ro</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First Time Trying Nail Art :) </t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft50ro</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1ft4kqx</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail Repair </t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft4kqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1ft3zzb</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Huge thanks to everyone on my last post who suggested their favorite baby pink, barely-there, milky, nude shades! </t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rdtqmvy5yzrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1ft2wy9</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Sea glass nails 🌊⚓️🐚</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft2wy9</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1ft2sh8</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this matte? </t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lvp2pgbipzrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1ft2rv2</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PPU quick dry top coat recommendations </t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ft2rv2/ppu_quick_dry_top_coat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1ft2pww</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>What am i doing wrong? Builder Gel keeps lifting at the free edge</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ft2pww/what_am_i_doing_wrong_builder_gel_keeps_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1ft1roy</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Jewel Beetle</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft1roy</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1ft1q59</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloweeeeen! </t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft1q59</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1ft1o4x</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phew! First time double stamping and first Halloween manicure! I'm pretty happy with the outcome. </t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft1o4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1ft1gwp</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Reviving thermal polishes</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ft1gwp/reviving_thermal_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1ft13lm</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Cosmic Cattitude</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft13lm</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1ft0dpa</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Secret Base</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i547bvxs7zrd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1ft0bfq</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Nail Polish FOMO</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ft0bfq/nail_polish_fomo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1ft06uq</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Juicy jelly </t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/afdrsdtl6zrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1ft06si</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Baby boa nails... ILNP Toasted, Moon Sugar Decals</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ft06si/baby_boa_nails_ilnp_toasted_moon_sugar_decals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1ft01ks</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t xml:space="preserve">✨ Your sign to get some Sassy Sauce Polish!! ✨ </t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gplr8oyi5zrd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1fszv7v</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Looking for a little help from the experts</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fszv7v/looking_for_a_little_help_from_the_experts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1fszh91</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Autumn nails </t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fszh91</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1fszdwz</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Merkitten 🩷💖</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fszdwz</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1fsz3c7</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>What colors would suit me best?</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nz4bz0tryyrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1fsyvmu</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Skittle Help? </t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fsyvmu/skittle_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1fsy4lo</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Glow in the dark polish available in the UK?</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fsy4lo/glow_in_the_dark_polish_available_in_the_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1fsxc3r</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Shorty September manis</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fsxc3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1fsx9ej</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>What happened with Cracked Polish?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ux6k4ydelyrd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1fswsj7</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>“Lightfast” 😍</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/chs49verhyrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1fswmam</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>My Nails are a BEACON 🚨</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fswmam</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1fswj1h</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>New week, new colour!</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zkwx0kpmfyrd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1fsw760</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Every polish I wore in September+ reviews ✨</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fsw760</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1fsw1wi</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Is there a way to cover medicine-induced nail ridges?</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fsw1wi/is_there_a_way_to_cover_medicineinduced_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1fsvsm2</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>First PPU order mani!</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fsvsm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1fsuqz7</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>ILNP Bare</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fsuqz7/ilnp_bare/</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1fsubyq</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Feelin’ a little batty 🦇</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fsubyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1fs47ph</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Bubbles in the polish</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fs47ph/bubbles_in_the_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1fstwde</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Starrily Wizard Duel Chrome</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fstwde</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1fstwcn</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>ILNP Coven: Sabrina</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fstwcn</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1fstuxm</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>First time trying Jade jelly</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fstuxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1fssk1n</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>My new go-to chrome nail look</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fssk1n</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1fsrx46</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fsrx46/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1ftfqvl</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Skipped fall and jumped right into Halloween! </t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftfqvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1ftfkok</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Last set til spooky season</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v25lz5vsm2sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1ftebju</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>My best acquisition of this month 💅🏻👑🩷🧚🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40ay7j2ea2sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1ftdwmc</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails of the Month </t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1fv2hhf62sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1ftdb6c</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Chisme nail art 💅</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2qgh6pzs02sd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1ftcnqn</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Tried doing a milky pumpkin nail!🎃 would love feedback/suggestions!</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/00468tfyu1sd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1ftcj30</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Trying to get better at 3D art :)</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftcj30</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1ft9kcy</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Intensely nails</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft9kcy</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1ft9cr3</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>pink press ons</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft9cr3</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1ft6g3t</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Kinda in love with this set honestly....</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pibjfu4g0sd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1ft6d4k</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aztec calendar nails </t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uyi8jf6jf0sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1ft630k</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Ghosts!!!!</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/op3lwcdbd0sd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1ft2n31</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Cinnamoroll 🩵</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9c60wfeozrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1ft17kf</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Sweetiepie nails</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ft17kf</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1ft0w7j</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you need 3D jelly to do this, or can you use white gel polish? </t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/DAW0H7NMGq3/?igsh=ZDExZXh0bnc2c2xj</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1ft0keo</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Stilettos</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ik83m9e9zrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1fsvynx</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>A little Halloween vibes for you</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fsvynx</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1fsus5c</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Does anyone know the original artist?</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fsus5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1fsseq9</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Some basic nail art problems I wanna ask</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/70i4ycx2dxrd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Oct  2 08:10:35 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_06.xlsx
+++ b/data/collected_data/2024_10_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C479"/>
+  <dimension ref="A1:C674"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8576,6 +8576,3321 @@
         </is>
       </c>
     </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1fub2sr</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>My first attempt at 3D nail art🎀</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fub2sr</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1fua9dm</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Green nails by me</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fua9dm</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1fu9lct</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Beautiful 😍🩵</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exh2bjydcasd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1fu99ot</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Is a nail lamp an appliance?</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gommpef98asd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1fu93on</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Spooky Chrome Spider Web Nails 🕷️🕸️</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4c2bqrc26asd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1fu8uvb</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu8uvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1fu8q0t</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>essie’s gel nail polish in matter of fiction 💅🏼🤍🎀</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9eq1xvuh1asd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1fu7qw0</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Spooky Szn</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9ozn5ucq9sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1fu7mq9</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>my first ghostface set! 🖤</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hopg21y4p9sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1fu7eza</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Cleanest option for longer nails?</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fu7eza/cleanest_option_for_longer_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1fu76yt</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>here’s the damaged nail that i mentioned in my previous post</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/087oe9bnk9sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1fu6o7z</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>First time ever doing nails!</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1eiberkff9sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1fu6juz</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Miss having my nails done🥺✨</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekzx2zx9e9sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1fu67q0</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Doing your own gel nails… worth it?</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fu67q0/doing_your_own_gel_nails_worth_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1fu63vk</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>glow in the dark nails for the first week of october🧪🌟</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu63vk</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1fu4pgz</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Just another October 1 post 🐍</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ccmt2bryw8sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1fu3qzz</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Periwinkle Chrome Mermaid Vibe</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu3qzz</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1fu30rw</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Is a 120 watt UV lamp safe?</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fu30rw/is_a_120_watt_uv_lamp_safe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1fu3nn7</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>my first time doing press ons and i LOOOVE them &lt;33</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu3nn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1fu2nga</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Some of my recent work!</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu2nga</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1fu2ker</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>I’m still in love with this girls</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qgyb1esyd8sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1fu2byh</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>The thumb wasn’t the best but still wanted to share🤗</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3e6ab5xb8sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1fu261z</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ready for Halloween 🩸 </t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu261z</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1fu1ohl</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Help with ideas!</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fu1ohl/help_with_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1fu1a39</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Did my nails the other night! thoughts? what can i improve on? (i used eyeshadow for the ombre)</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu1a39</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1fu18il</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Beetlejuice Beetlejuice Beetlejuice</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu18il</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1fu0mu3</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>What do You think of My new Nails?</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5adn1mszx7sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1fu0hie</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>cowgirl but make it spooky</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mvrvlqbtw7sd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1fu0ffj</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>My 4th time doing my nails with Luminary. Happy Fall, y’all🍂👻</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cgfy887dw7sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1fu0dl0</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Howd I do?</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu0dl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1fu09mj</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Where to find full coverage tips for wide nails</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fu09mj/where_to_find_full_coverage_tips_for_wide_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1ftzs4k</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Already looking for chrome inspo pics for my next set</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fq7kxv1er7sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1ftztx6</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>First set of Halloween season</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftztx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1ftztpw</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>...uhh... meow? 🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftztpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1ftyrxr</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>First time wearing gel x</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xqsrlqwpj7sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1ftzblq</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Pumpkin patch nails</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eoowtdxvn7sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1ftz5ok</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>I'll always love a classic short natural pink nail😍</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftz5ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1ftz3um</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>[Seeking Opinions] Had my nails done for the first time in 4 years. Unsure about the color.</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftz3um</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1ftynq6</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Hiya! Something super simple today. But I am excited to say I'll be filming the painting of a full set! Wish me luck on my first time!</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/403lldski7sd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1ftydpw</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Done these tonight as it’s now October! </t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a3o2e61tg7sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1fty9uq</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>My 4th set learning gel polish</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fty9uq</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1ftxphx</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky Season Bat Nails! </t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ru3z2ruub7sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1ftxmiu</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t xml:space="preserve">16 hours of painting. Worth every minute in my eyes. Little roadrunner was probably the hardest and then by the horses and air balloons. My first of many desert sets I'm sure. </t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftxmiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1ftxf0g</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>My nail tech never fails</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftxf0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1ftwsbf</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Can I get an acrylic with a damaged nail?</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ftwsbf/can_i_get_an_acrylic_with_a_damaged_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1ftws3g</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Did this gel set on myself (still learning) 💕</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hdw7wsc457sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1ftwej8</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Russian/Structure Manicure</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ftwej8/russianstructure_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1ftwai4</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>New set and I love it!</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ajq93djj17sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1ftuzs9</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>New set 🧛‍♀️🩸♥️</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftuzs9</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1ftw370</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Been really working on growing and shaping my naturals. No tips 💕</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftw370</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1ftvey9</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>what can i do to this set to make it better 😭</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ykhs66bv6sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1ftv2al</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These were so beautiful but they didn’t last, it was hard gel and they started breaking and lifting a few days after. But aren’t they so pretty. </t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9yid9qqs6sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1ftuxmr</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Builder gel </t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ftuxmr/builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1ftuqxv</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>🩸</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytlz0w8eq6sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1ftupcc</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Is there a way to easily chip your nails?</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gamanhv2q6sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1ftuobm</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Boo! Happy October!</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9s7abpfvp6sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1ftul3u</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>ILNP - Amped</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftul3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1ftu4ey</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Happy october 🙆🏼‍♀️</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26ddkc0vl6sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1ftu3b9</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>It’s finally time for spooky nails! ☠️🖤</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o87mpc0nl6sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1fttroe</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>First time doing my own acrylic, and I’ve got questions</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/muwtsdnbj6sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1fttpci</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t xml:space="preserve">milky (?) french tips! what do we think </t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fttpci</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1fttlvo</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Eye Five</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/05ztnta4i6sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1ftoqd0</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Now vs 1 Year ago</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftoqd0</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1ftnfgo</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>How can I fix these nails</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftnfgo</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1ftta6f</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Are these too boring/basic?</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ej9dqg6sf6sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1ftq1li</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t xml:space="preserve">did my nails for the twentyonepilots showthis weekend! </t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftq1li</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1ftrgfi</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Eggshail nails, shaping tips?</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u315f6ve26sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1fts4w1</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Happy October 💅🏼🖤🎃</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fts4w1</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1ftsykg</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Press on improvement</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ftsykg/press_on_improvement/</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1ftsspv</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>My new nails are very cute 💕</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1moeas1bc6sd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1ftsl71</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>In love with pastel pink 💅💓</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ithzuq1ta6sd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1ftsjtb</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Still love the colour, quiestionig the shape</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u8xx9t1ja6sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1ftsjea</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail polish, oil on canvas board </t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2rvyw5xfa6sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1ftsbhy</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>DIY Nails</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5313694u86sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1ftrvdv</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A little break from gels </t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftrvdv</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1ftrt2b</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Had to cut them short for pottery but I love the color!</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/170ex8u356sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1ftrifv</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>My nail tech kept giggling at how cute the frog is! 🐸</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tiptiw5u26sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1ftrhlb</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>It's been a decade since the last time</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftrhlb</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1ftqw1k</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t xml:space="preserve">junk nails set i did yesterday on myself </t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsto65k7y5sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1ftqt9y</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> mermaid nails for the Chappell Roan show 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftqt9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1ftqls3</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beginner question!! </t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ftqls3/beginner_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1ftqgxh</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Vampy red and black for the start of October 🩸(OC)</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/83b3mtk1v5sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1ftqa5s</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>DIY Press-ons!</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5x3ahvwmt5sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1ftpqcc</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>I so proud of my ombre pink/blue gel tips</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftpqcc</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1ftpmpy</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on advice please! </t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ftpmpy/press_on_advice_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1ftpj0t</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Love the color shift</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9phur3mxn5sd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1ftphkd</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Love the color shift!</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftphkd</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1ftpasr</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Some ghost for Halloween</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lvu1nei7m5sd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1ftp8ty</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>That purple cateye 😍</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftp8ty</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1ftp1fa</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Loving these ✨✨</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftp1fa</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1ftnwny</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>I love my Current Set!</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftnwny</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1ftn6ae</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>First ever press ons!</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftn6ae</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1ftmx59</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bats and Gouls, oh my! </t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftmx59</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1ftmnyr</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>How do people wear press on’s with sticker glue?</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ftmnyr/how_do_people_wear_press_ons_with_sticker_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1ftm3c1</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In love with this colour ❤️ </t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftm3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1ftlyqf</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail twinsies </t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tw4dbyect4sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1ftlvzu</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t xml:space="preserve">do these scream press on nails </t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftlvzu</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1ftl3uq</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Witchy for October 🎃</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dzm3veo0k4sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1ftk92q</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Does the 3D flower not match the rest of my nails?</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftk92q</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1ftk1eh</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you wear your own press-ons?  </t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vheaqbxq64sd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1fu9sq4</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Such a cool polish!!</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu9sq4</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1fu9ncb</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Fall mani</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu9ncb</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1fu940l</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red black skittles </t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu940l</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1fu8tye</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Where can a Canadian get an affordable paddle brush?</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fu8tye/where_can_a_canadian_get_an_affordable_paddle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1fu815a</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Matching hair and nail combo</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu815a</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1fu76c1</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ghosted </t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu76c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1fu748o</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Olive &amp; Sage green press on set for fall 🫒 </t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu748o</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1fu66xp</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In love with Iris! </t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu66xp</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1fu5zvc</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How can I stop the bubbles? </t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5zzv78g099sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1fu5dp3</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A month of manis </t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu5dp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1fu5beq</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Hello laqueristas! Polish recommendation for this shade? NOT navy please! Ty! 💙</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwf85l7r29sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1fu583t</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Scored 134 bottles of polish for $100 on Facebook. Don't normally do multi colored manis but I'm gonna have to for a while!</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu583t</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1fu54r3</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Please share your favorite polishes for magnetizing in the velvet style because I’m OBSESSED. </t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rq5hvuzz09sd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1fu4xb7</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>solo mission by holo taco 👩‍🚀🎀</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eefemsc0z8sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1fu4iil</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>I’m im-pressed 💅</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1cjw86d5v8sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1fu472u</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween Vibes 🎃 </t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ky5jsz38s8sd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1fu4266</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I think this is my favorite polish combo so far! </t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu4266</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1fu3uld</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>The perfect fall red 🍂🍎</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu3uld</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1fu3li3</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>(Gifted PR/ad) ILNP Coven: Ritual</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu3li3</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1fu3a3e</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Found ILNP dupes in a Mexican brand. </t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvl88iy3k8sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1fu39c2</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>I'm gonna miss having nails like a fairy queen, I've made the big chip, and now I'm ready to play BG3 and write fanfiction! Looking forward to my first blind playthrough :)</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu39c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1fu34ug</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Had to bail out a sinking (ghost) ship</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu34ug</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1fu30rl</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>This thermal is so special 🤯</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu30rl</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1fu2jsu</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Why do they use the led lights on regular polish?</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fu2jsu/why_do_they_use_the_led_lights_on_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1fu2cl8</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>First Spooky Mani Of The Month!</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu2cl8</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1fu22i4</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Sour Apple Rings w/ Swamp Puppy</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu22i4</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1fu1ru1</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Probably my favorite nail combo yet!</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu1ru1</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1fu1e1x</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>What I wore in September</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu1e1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1fu0ucv</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>ILNP spiced cider 🍂🍺</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu0ucv</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1fu0kif</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Finally found my perfect brown!!</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu0kif</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1ftzn7p</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Spooky season commence!</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/va9uwtzaq7sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1ftzm4s</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Don Deeva Le Tit Snow</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftzm4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1ftzf1m</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Helene </t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ftzf1m/helene/</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1ftzeuo</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Mooncat Jewel Beetle</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftzeuo</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1ftz65v</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The many faces of psilocybin </t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7nq4jnyom7sd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1ftz67h</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Top 3 favorite indie polishes ever?</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9eb0cfrm7sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1ftz4ds</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The amazing Psilocybin </t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/37o2154cm7sd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1ftyf7s</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Couldn't decide which of these two options to go with for my first fall manicure, so I just did both!</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jedfh44h7sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1ftxmp8</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Willis skittle </t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/srlpumbab7sd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1ftxf0d</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Spiced Cider by ILNP</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/snahzorp97sd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1ftxccg</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Removal help</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ftxccg/removal_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1ftx7vf</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Psilocybin Help!</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ftx7vf/psilocybin_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1ftwzbn</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Labradorite in polish form!</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftwzbn</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1ftwoms</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Emily de Molly Always Around Me + Sally Hansen Let’s Get Digital</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cbf2v52f47sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1ftwljb</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Cozy velvet nails</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ds7su6ur37sd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1ftwiy8</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BKL- Proof of the Afterlife </t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftwiy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1ftptx2</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Proposal Polish?</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ftptx2/proposal_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1ftw77q</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Purple with green/blue shimmer: a comparison</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftw77q</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1ftv7e1</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>month of manis: september</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftv7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1ftum5j</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>ILNP - Amped</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftum5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1fttmvd</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Can you develop allergies to non-curing nail glue?</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fttmvd/can_you_develop_allergies_to_noncuring_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1fttmd1</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Polish or Don’t Polish Peeling Nails?</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fttmd1/polish_or_dont_polish_peeling_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1fttdp2</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Help identifying an old opi bottle</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4v1uis6ig6sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1ftsyxu</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Under nail magnet works some days but not others?</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftsyxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1ftsehb</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>What is this???</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftsehb</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1ftro7w</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>October Vibes</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7x93yqb046sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1ftrkno</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Original Cindy by Emily de Molly light blurple dupe?</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ftrkno/original_cindy_by_emily_de_molly_light_blurple/</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1ftrcrz</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>The Inspiration, A Fancy Salted Egg Custard Bun VS The Nail Art</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j44yxt7n16sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1ftr3g5</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Cracked Polish is 🔥🔥🔥</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftr3g5</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1ftq9rk</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Wish me luck with my big interview today! 🤞</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftq9rk</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1ftpwls</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>What color should I paint my nails with this outfit? Help.</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vjpdshuq5sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1ftpwe9</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>And Old Favorite</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7iy57wsq5sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1ftpu9w</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did twentyonepilots nails for the Columbus show this weekend! </t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftpu9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1ftpg95</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>This centipede…is a predator 🐛</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftpg95</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1ftoe15</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>first at home gel mani</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftoe15</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1ftoc15</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>What are you doing in my swamp?</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftoc15</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1fto0e1</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Heartbreak</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fto0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1ftnxv4</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>purple and ready for fall 💜</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftnxv4</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1ftn81f</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>(Gifted PR/ad) ILNP Coven: Moonlit</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftn81f</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1ftkpvp</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>ISO: shimmery, indigo based magnetic with a lime green pull</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7f0eygndf4sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1ftkfpt</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>PPU Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ftkfpt/ppu_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1ftk719</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>my nails match this bottle of benadryl 💖💅😂</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftk719</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1fu8m8d</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>First attempt at zodiac nails for (Libra szn)</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu8m8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1fu81ar</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>What do you think</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnuobr3ht9sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1fu7gwa</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Halloween model 👻</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu7gwa</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1fu7413</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>A cute little space inspired set. Looks like jewels!</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu7413</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1fu5wxc</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Spooky nailssss</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu5wxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1fu3pcl</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Más chrome nail art</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5it73n5tn8sd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1fu3oid</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Periwinkle Chrome Mermaid </t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu3oid</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1fu3oa9</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Some sets I made for spooky season! 🎃</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu3oa9</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1fu2ti6</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Help with ideas!</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fu2ti6/help_with_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1fu2b7m</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Spooky but make ot pink</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lu8oleqb8sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1fu25b9</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My gf did these </t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fu25b9</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1ftzwpd</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Halloween nails #1</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftzwpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1ftzl4z</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>nails to match my dress</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftzl4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1ftz29d</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Hiya! Something super simple today. But I am excited to say I'll be filming the painting of a full set! Wish me luck on my first time!</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5v0udacql7sd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1ftz0it</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>My take on the tortoiseshell trend 🖤🤎🧡</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/krvqpkejl7sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1ftwpl2</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>I’m obsessed 🤎👻🌸</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhvw6t6l47sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1ftw9th</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>In honor of October, my very first nail design vs now</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftw9th</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1ftvpcp</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Honest opinions. </t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftvpcp</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1ftru57</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Happy October 💅🏼🎃🖤</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ftru57</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1ftpnpz</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>The set I did on myself😭💅🏽</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qrniroqxo5sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1fto9xv</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Fall Nails</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fto9xv</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1fto9ui</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beginner fall/halloween nails </t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5p68b12e5sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1ftlo2s</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>I’m lactose intolerant (I love milk)</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rat9el6q4sd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Oct  3 08:10:37 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_06.xlsx
+++ b/data/collected_data/2024_10_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C674"/>
+  <dimension ref="A1:C853"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11891,6 +11891,3049 @@
         </is>
       </c>
     </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1fv1ik5</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>My favourite ones yet</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bvf6gnv6khsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1fv1hr6</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Gush over this cutest set with me 🍄</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fv1hr6</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1fv1dc2</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Second pair of acrylics (PVC)? Ever. Got these bad boys in Thailand for $25 while visiting husbands family.</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fv1dc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1fv1c0b</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Can I use a regular nail polish color with a gel clear coat?</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fv1c0b/can_i_use_a_regular_nail_polish_color_with_a_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1fv0z4m</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>halloween?? nails</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aejjpb8ddhsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1fv0gdo</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my nails done on vacation in Taipei. I think they are so fun </t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fv0gdo</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1fuz34z</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Should I work my way up to longer nails?</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fuz34z/should_i_work_my_way_up_to_longer_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1fuzcco</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Question about powder acrylic</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fuzcco/question_about_powder_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1fuz5nq</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{PR} Halloween hand painted ghost nails </t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuz5nq</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1fuz36l</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>new set by my friend !!</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuz36l</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1fuz023</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Getting started is overwhelming </t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fuz023/getting_started_is_overwhelming/</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1fuyv2j</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>October Vibes !</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nofpthyapgsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1fuytd2</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>They be spooky like that</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvi5impiogsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1fuyeso</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Flashy cat eye claws for the start of October 💅🏻✨✨</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuyeso</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1fuy8d2</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails for October </t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q74qbqlvigsd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1fuy821</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Go-to cuticle oils?</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fuy821/goto_cuticle_oils/</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1fuxtlr</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My ocean set 🪸 🫧 </t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/by1bh32uegsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1fuxop1</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Finally time for spooky season nails!</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwdtuviidgsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1fuxjau</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set I did! I was going for a red jade look. Mixed my own “jelly” red </t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuxjau</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1fuxhp0</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Looking for a charger replacement for this specific drill, any help appreciated!!!</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hgo7t05nbgsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1fuxd3l</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>💜✨</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ez6mtxscagsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1fux3iv</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Fall chrome✨</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fux3iv</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1fux185</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>New design today! I absolutely love!🎀</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8u0bwvca7gsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1fuwz6r</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Birthday Nail Set 🤍</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuwz6r</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1fuw6pf</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glass chrome french tips </t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/et9mf73hzfsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1fuvxi3</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Wedding nails</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuvxi3</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1fuvsg8</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>I can’t stop staring at them🤩</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/alwun8evvfsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1fuvmzo</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple, not perfect, nails done at home. Light pink, with design. </t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuvmzo</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1fuvf5w</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>How to get nails to last?!</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fuvf5w/how_to_get_nails_to_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1fuvar2</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are the European girlies wearing? </t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fuvar2/what_are_the_european_girlies_wearing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1futno7</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some designs I created today now I don't know which one to choose! </t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1futno7</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1fuuefw</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you think french nails are boring? </t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ud5c4d0ejfsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1fuu7ap</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got some autumn themed nails yesterday </t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lty2piomhfsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1futwcj</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Nails </t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1d8o4pe0ffsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1futnmg</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Pedi</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n73708cxcfsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1futlkl</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>👽🪐🌙</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1futlkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1fusxs2</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Tried something new today</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zh195nxc6fsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1fusfn8</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t xml:space="preserve">After years of biting my nails, I finally stopped and got them strong and healthy! Never knew how much nail oil really helps. I was painting them but they started getting yellow so now I just use a clear base. </t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7f421mup1fsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1fus8gu</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Basic Fall Set 🍂🍁</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fus8gu</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1furygh</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Product for preventing breakage in long natural nails?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1furygh/product_for_preventing_breakage_in_long_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1furdi1</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Inspired by another post, my halloween nails</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mlcjup5htesd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1furgob</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>🤍</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1furgob</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1fuq6as</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>What to do for wedding nails when I have a gel allergy?</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fuq6as/what_to_do_for_wedding_nails_when_i_have_a_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1furec4</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Purple 💜</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dypnxibntesd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1fur5lp</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Halloween scream nails</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fur5lp</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1fuqej1</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any ideas how to stop this from happening? </t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuqej1</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1fupo8a</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Nails okay, and studies always up to date!</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xl9fipemgesd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1fupn82</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Before and after ✨</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fupn82</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1fupf5a</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>My fall set!</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ailc9dqeesd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1fupesx</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>New BIAB set 💥</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxs8f8goeesd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1fup90u</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Working Gals Nails?</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fpc24qpfdesd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1fup2ts</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Nails for my upcoming Disney trip</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fup2ts</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1fuouv5</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Brown w chrome 🤎</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03i6h7kfaesd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1fuoscu</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>how to make gel x last longer</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fuoscu/how_to_make_gel_x_last_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1fuoktd</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Halloween nails</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuoktd</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1fuog8z</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween BIAB 🎃 </t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tep8noxc7esd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1fuod0z</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Is my left hand pointer finger crooked? Just got these done and I’m trying to not let it annoy me lol</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuod0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1funt2p</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Acrylic, Dip, Gel, GelX?</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1funt2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1funj4u</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Personally, I hate the flowers</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1funj4u</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1funuih</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Working on my at-home gel extensions!</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1funuih</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1fuo7yi</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday Nails </t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuo7yi</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1fuo3yb</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Halloween Nails for the first time!</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/up31uz6t4esd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1fuo3gf</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Framed Fall 🍁🍂</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uboe46wp4esd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1funw91</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>I've been doing nails as a profession for almost 4 years. Why does it take me so much time after all these years?</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1funw91/ive_been_doing_nails_as_a_profession_for_almost_4/</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1fun8nz</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>New babies 💅</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fun8nz</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1fums2y</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>I made myself a metal press-on nail</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fums2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1fumpwt</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>For my bestie!</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fumpwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1fum1ky</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Flashy palette cleanser</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fum1ky</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1fulxhz</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>What about this for halloween?</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1sr0q4podsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1fultok</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Fall sweet fall</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fultok</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1fulpgb</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Hurricane Helene Destroyed My Town - Best Way to Take These Off ?</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m82vltm2ndsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1fujg9q</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>My first ever matching Mani Pedi</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qu3i9q3t6dsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1fulj78</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Spooky Nails</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8t3htjltldsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1fulikx</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Which colour?</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fulikx/which_colour/</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1fulgmi</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>DND Gel Appreciation</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mykixk0aldsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1fula2p</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>{PR} Shockwave by Sassy Sauce Polish</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fula2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1fukt44</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Are these that bad? She went home and immediately soaked them off</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fukt44</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1fuk5fm</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Does this base color work with my skin tone?</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuk5fm</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1fujlfu</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Fall Nails</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fujlfu</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1fujhf6</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are these awful? </t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fujhf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1fuj5uk</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Gave my nail artist free reign, just asked for turquoise &amp; purple chrome &amp; some details of whatever she wanted. I'm in love 😍</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6h7zxgtn4dsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1fuixy5</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>I think my nail beds are finally growing out, bare nails here I come!</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bodzuoq03dsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1fuioyo</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Forever press on obsessed </t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tl7q94y51dsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1fui6xb</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Yellow/white &amp; Nude/Yellow french tips</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fui6xb</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1fuht16</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>painting over gel nails</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sg52k8miucsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1fuhrbz</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are my nails to healthy </t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fuhrbz/are_my_nails_to_healthy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1fuhosb</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>October nails</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4bwx71bmtcsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1fuhkzv</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Who else is a big Disney freak ?😍 love it or not</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hq5no7btscsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1fuh1fa</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Cateye set, on myself ✨️</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuh1fa</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1fugwtl</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Opinion on 3D gels?</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fugwtl/opinion_on_3d_gels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1fug7sx</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Cat eye on burgundy polish 💖✨️</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y5imdk9rhcsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1fug4wm</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set! </t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/026hryj2hcsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1fufe3i</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Blue Back cat eye nails</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fufe3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1fuf2i6</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Silver cat eye in natural nails 🪩</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yurm7t3q7csd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1fuezmx</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Is this because I cut my cuticles instead of pushing?</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuezmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1fuep68</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Dark Wine Red Nails with Chrome :D</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuep68</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1fue51q</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>I love my manicurist because he exceeds my expectations every day🤩</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8lo7xgfybsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1fuds7v</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween ready! </t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5fpg0s01vbsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1fudkh6</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Another day, another glitter!</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lz895x7tsbsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1fud7fb</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>My fav nail art ✨🌟</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bvg2s7jpobsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1fv24mr</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Spooky season is here</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dbfjzjdfshsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1fv0ui9</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Nails Inc is so underrated!</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fv0ui9</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1fv0l0t</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Sometimes what's simple comes out the prettiest</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efa5oro68hsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1fuzv90</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t xml:space="preserve">orly bare rose + revlon top coat :) </t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1kyu2gt00hsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1fuzuay</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>my nail polish swatches!</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/auwcd2fpzgsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1fuz4gb</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{PR} Halloween hand painted ghost nails </t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuz4gb</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1fuxff6</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Great Lakes Lacquer | Never Trust the Living</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuxff6</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1fuw7ph</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>ILNP Velveteen 🩶💜🤎</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuw7ph</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1fuw70w</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>PPU arrived today and I am obsessed!</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bbupt7vjzfsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1fuv46e</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Rocking Horse Fly 🔥</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zzhysvunpfsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1fuusnw</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Storage ideas </t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ksbw9ojumfsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1fuul8c</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Beetlenails beetlenails</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qm7r0kt1lfsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1fuuehq</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>orange flakies ✨️</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuuehq</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1fuu9lz</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When You Match the Nails to The Book 💅🏻📚 </t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xbnlkdk7ifsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1futjip</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t xml:space="preserve">$20 Target Score!! </t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9sc2g07ybfsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1futi00</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>It's currently 106°</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1futi00</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1fut2fm</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Cirque Colors</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jbxz5sxi7fsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1fusynq</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Take It or Leaf It!</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fusynq</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1furul6</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Another Clionadh stunner.</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vyiwjff2xesd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1furgt1</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>September PPU was dangerous</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1furgt1</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1fuqtft</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Had to show off my nails today, I’m star struck by the colour and the rainbows! Cupcake Polish</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuqtft</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1fuqscu</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>opinions on JINsoon?</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fuqscu/opinions_on_jinsoon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1fuq6tw</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Down down the witches road</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wac8qmkkkesd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1fupzj4</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I would lay down my life for jelly polishes </t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fupzj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1fupv3w</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I think these are the best nails a 3 year old has ever done.  </t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k3cuefk2iesd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1fuptbg</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Halloweeeeeeeeen</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9u7vdixohesd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1fupl53</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Velvet psilocybin </t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/warm8dzvfesd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1fuoxc3</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Flakies + matte my love ✨</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuoxc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1fuoaju</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Starting October off with vampy vibes 🩸 </t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuoaju</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1fun24n</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Are there any dupes for spirit fingers?</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5gxtazbxwdsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1fump4u</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>First stab at velvet effect with 22 lb alnico horseshoe magnet. Details in comments</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zpsa20cotdsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1fumntt</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Update on my skin tone matching woes</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fumntt</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1fumnb7</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Miracle Gel on Clearout 🇨🇦</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ev6087zztdsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1fumcxf</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Beautiful Garbage</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fumcxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1fulxq8</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Raphael 🪽 </t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fulxq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1fulbdc</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Redemption Arc: Rotten Bananas Becoming Bread - Death Valley Nails</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fulbdc</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1ful8bq</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>{PR} Shockwave by Sassy Sauce Polish</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ful8bq</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1fuktp4</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Yellow PPU Skittle</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuktp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1fukiui</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Loud Lacquer- Party Monster</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fukiui</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1fujni0</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Top three brands</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fujni0/top_three_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1fujf3r</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Matte Top Coat</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fujf3r/matte_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1fuj6jt</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>feelin’ very fall 🍂</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuj6jt</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1fuj4e4</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Trying to figure out what neutral nail colors look good on my skintone! Ive always had a hard time with that.</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dajbr2wwzcsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1fuiihv</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Sassy Cats Lacquer - Who You Gonna Call?</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuiihv</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1fuhd9c</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Potential allergy </t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fuhd9c/potential_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1fuh8mt</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Magnetic polish tutorials </t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fuh8mt/magnetic_polish_tutorials/</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1fuh1u2</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>I think I’ll  have to join the shortie gang for awhile</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qasu0vsmocsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1fugqk1</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Pls ignore the pillow wrinkles in my topcoat. I did my nails before bed and sleep like a cartoon baby.</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fugqk1</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1fugppj</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>ILNP Olive Grove</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fugppj</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1fufkup</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Nudes game matte/glace</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fufkup</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1fufc78</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Shimmery turquoise dream</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fufc78</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1fuf893</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>First try trying something different on the tips, glitters are forgiving</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mq7ozsov8csd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1fudzpq</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Fall Flakies!</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4c6mp63xbsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1fudx47</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t xml:space="preserve">September manis: looks like I’m taking the long way around to fall colors this year </t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ro4qocykwbsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1fud4ec</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What should I do? It’s really painful </t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fud4ec/what_should_i_do_its_really_painful/</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1fube6f</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PSA: found a great primer 🐐 </t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fube6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1fub6z7</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Saving money</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fub6z7/saving_money/</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1fub5uk</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Witchy tango</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bfjstjwjxasd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1fv2md6</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>My first attempt, how did I go?</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/scf4qkoqzhsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1fv29dd</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>First time using a cat eye gel</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k31jprwhuhsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1fuz9v0</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel-X &amp; Dip 👻🎃 </t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuz9v0</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1fuxbec</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>what gel for 3d designs?</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fuxbec/what_gel_for_3d_designs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1fuw6gh</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Halloween nails - glitter encapsulation with pink bottoms! What do you think</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuw6gh</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1fuw2ni</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t xml:space="preserve">a blue set by me </t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuw2ni</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1fuvlwx</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Today’s set 😻</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tdj7y527ufsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1fut85l</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Created these today and now I can't decide which one to use.</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fut85l</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1fuqugb</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Stitch and his girlfriend's nails</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dj4f00uipesd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1fuovzv</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Halloween Vibes</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/en613vznaesd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1funaf0</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>New babies</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1funaf0</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1fumb2a</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Fall sweet fal</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fumb2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1fug8rg</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on set </t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/99ynfdakhcsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1fujdey</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holding on to Summer! (Done at Bea Beauty, Dublin, Ireland) </t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/enps2z186dsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1fuir0o</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Nails delicate but elegant ones from the best manicurist by: vero di palazzio</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fuir0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1fuh7ar</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beautiful tone in nails by: michael tran </t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfj8nttupcsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1fugghe</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>💜💜💜</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vfr5b36tjcsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1fug9q2</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall theme </t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fug9q2</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1fufrbt</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Overlay frenchies</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fufrbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1fuc1ix</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>did my nails while watching a lecture</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tf7nwevs9bsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1fub8z0</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Share an easy way to make chrome nails</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bn15vibgwasd1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Oct  4 08:10:43 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_06.xlsx
+++ b/data/collected_data/2024_10_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C853"/>
+  <dimension ref="A1:C1047"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14934,6 +14934,3304 @@
         </is>
       </c>
     </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1fvttd3</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which one would you pick? </t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvttd3</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1fvts54</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Unprepared for SATs but at least my nails look pretty :)</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/81kvxyke2psd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1fvtrhn</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>What are your "sluttiest" nails?</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fvtrhn/what_are_your_sluttiest_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1fvt96d</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails 💅🏼 👻 </t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvt96d</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1fvsziu</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>French Tip Ghost Set 👻</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvsziu</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1fvst44</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! </t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gy3to725posd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1fvs6tw</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>All ready for spooky season</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bzd9k1oahosd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1fvs61h</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Square set </t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvs61h</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1fvrw85</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>HR Giger / Alien nails</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvrw85</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1fvrpyi</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Haloween nails!! 🎃</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e3pbia1fbosd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1fvqmbz</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gore nails for Halloween 🎃 </t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gh4dramxynsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1fvqmxw</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Jujutsu Kaisen x Mochi Donuts!</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvqmxw</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1fvqmu3</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it too early for something festive? </t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dkfqir2znsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1fvqmmc</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Made my first full boo set</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vilcuro0znsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1fvqgp9</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>A bit early for Santa nails? lol</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/45wdp1mcxnsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1fvqfrh</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>My first acrylics I did, a few years ago 😅😂</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rmofvlv2xnsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1fvqdub</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SpongeBob Halloween set I did! </t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vnlul9mhwnsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1fvqciw</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky season nails </t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hvfae1k3wnsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1fvoapi</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>[Natural Long Nails Hacks]</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fvoapi/natural_long_nails_hacks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1fvpw2l</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>My Birthday/Halloween Set</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvpw2l</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1fvppbq</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Scorpio Seduction non-toxic alt? </t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tcaiv7qgpnsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1fvpmau</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inspired my one of my favorite plants! </t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vb4wr7xmonsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1fvp66p</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Russian nails</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvp66p</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1fvp13y</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Halloween Frosting Set</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvp13y</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1fvoypo</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>New set. I let someone pick the dip.</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzb8gvt8insd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1fvoobo</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Chrome shine</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvoobo</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1fvoml9</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Always Red ❤️</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nuzgsez0fnsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1fvofwb</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>How to clean up the surrounding skin?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rnlgwo7adnsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1fvo0h3</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t xml:space="preserve">simple and cute HK Halloween nails </t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvo0h3</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1fvnv3c</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I made press on nails. I don’t know how much to charge. </t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zd89vl6u7nsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1fvnime</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Yummy rilakkuma 🧸🍦🎀⭐️</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iaz56wxl4nsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1fvnfcx</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween Freestyle </t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvnfcx</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1fvmzov</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Nails done for the first time</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvmzov</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1fvmmy5</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Cat nails Halloween edition</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dm2zcrujwmsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1fvm25u</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beginner questions </t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fvm25u/beginner_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1fvlyi5</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>It girl nails 💕💋</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rj8z3tbkqmsd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1fvlgrn</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>How soon can I remove a fresh set?</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fvlgrn/how_soon_can_i_remove_a_fresh_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1fvlf6d</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Spooky season nails 🕷️🕷️</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ds4y6bovlmsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1fvlejy</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Pink butterflies</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tuofiunqlmsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1fvl1ej</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Witchy Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvl1ej</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1fvl057</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Can we talk about REMOVING and refilling gel nails AT HOME?💅🏼🏠</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fvl057/can_we_talk_about_removing_and_refilling_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1fvkzt4</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matched my gel Polish to my autumn coat today. </t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yfgpfgs6imsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1fvk9rd</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Full cover gel tips, wide, sculpted (EU)</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fvk9rd/full_cover_gel_tips_wide_sculpted_eu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1fvk89e</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pastel vibes </t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvk89e</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1fvk7im</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Cutesy Dark Red 💕</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvk7im</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1fvj9rh</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I've never gotten a fill before, how long should I let them grow out? </t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rp51q4ww3msd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1fvk6br</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Last design for September 🍐</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvk6br</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1fvk40r</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>15M new to nails</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fvk40r/15m_new_to_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1fvk0hr</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Starting October off with the shorties 🍪</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvk0hr</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1fvjv5j</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>New Nails! Red Frenchies w/ Almond Shape</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/thb0s2sq8msd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1fvjpjy</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Decided to try growing out my real nails!</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zp1xr6rf7msd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1fvjmpl</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>first time in a year! 💫</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lsgv09ct6msd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1fvidjd</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Just learning to do nails on others, I start school in 6 months this is the 4th set I’ve done on someone else.  How do I get better at line art?</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/485t85luwlsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1fvi6c1</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>October inspired nails 🧡🖤🧡</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvi6c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1fvi78l</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Tortoise shell again but this time make them long 🤎💛🧡</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvi78l</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1fvio0h</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>How long to keep filling an acrylic overlay?</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fvio0h/how_long_to_keep_filling_an_acrylic_overlay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1fvj4n4</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wanted Something Different </t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y7ajp1hs2msd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1fvihjz</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>spooky nails 👻</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvihjz</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1fvi1b2</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>New gel set</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jgkvsko7ulsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1fvhrgv</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Nail polish</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/01q6lk74slsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1fvhjpm</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Saved by the bell!!</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvhjpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1fvhadq</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Damage rehab: Strengthener, oil, or both</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fvhadq/damage_rehab_strengthener_oil_or_both/</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1fvhem3</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Got my nails done for…</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvhem3</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1fvh9yf</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>🎀✨Yuuuuuuup</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvh9yf</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1fvh9pq</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Second time doing my own hard gel nails </t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvh9pq</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1fvh3hz</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>New to this, first time posting!</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d82hzqu2nlsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1fvgohg</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Getting back into it!</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0ld5onvjlsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1fvgnv3</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>black stiletto nails &lt;3</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvgnv3</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1fvgi47</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hi. I’m Ada, new to the nails community. I did this last year as one of my Halloween Nail Inspo. What do you think ?? 😊 👻 </t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4y2bo9jilsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1fvggjg</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>New Halloween Set</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ovandcl6ilsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1fvgclr</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Was going for a clean Fall vibe… did it come out more Spring than Fall though? </t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvgclr</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1fvg0cj</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>I'm OBSESSED with Frankie from ILNP</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvg0cj</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1fvf7ar</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Matte black for October 🎃</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjorizmj8lsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1fvf4g3</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Sanguine Lust Nails</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvf4g3</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1fvf1oc</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Buffing files similar to this one I already have?</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/587nvdwc7lsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1fvd9u5</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Fall/Autumn nails</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fvd9u5/fallautumn_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1fvdpmc</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>This years Halloween avocado nails! 🥑</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvdpmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1fveict</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Lunch Pose! (Bonus dog at the last 2 slides)</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fveict</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1fve7qo</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Autumn nails </t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93m38ab41lsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1fve6oh</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press ons 💅🏻 </t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fve6oh</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1fvdx6j</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>New nails of the month</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvdx6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1fvcvrm</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Candy corn nails</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7up1lrxqksd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1fvdujm</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally feeling fall </t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hgr3vv78yksd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1fvdtxd</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Nail broke today 🥲 Nail tech saved ne 😇💖</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvdtxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1fvdcyl</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My new elegant nails </t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j90vd0aiuksd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1fvd6hh</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is RARJSM reliable? </t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fvd6hh/is_rarjsm_reliable/</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1fvd5du</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Always red nails for fall </t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvd5du</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1fvd1yi</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween Nails </t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvd1yi</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1fvcslg</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Pink &amp; green 💚</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzinajp8qksd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1fvcrcz</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Wedding nails - help!</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kdkjs3xzpksd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1fuz3f9</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Help A First Timer!</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vj4fv51qrgsd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1fv1jd5</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Fall Nails 🍂</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fv1jd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1fvcar0</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>I left my Rhinestone Glue out in the SUN 😭</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ufwkbsjjmksd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1fvc30a</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love this colour! No filter, just Spanish sun! </t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qlt8baixkksd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1fv1b2l</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Linkin Park New Album Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jiycsqghhsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1fv5sie</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>e file bits</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fv5sie/e_file_bits/</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1fv6jvq</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Can you do aura nails with regular polish?</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fv6jvq/can_you_do_aura_nails_with_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1fv90vt</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Protecting natural nails from moisture</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fv90vt/protecting_natural_nails_from_moisture/</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1fvbf6q</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gorgeous Vacation Nails </t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvbf6q</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1fvbd9g</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Ready for Halloween!</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bck81ugleksd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1fvt3cc</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>super glowey shift ✨💖</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvt3cc</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1fvssak</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Dupes for Award For Best Nails Goes To... by OPI?</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fvssak/dupes_for_award_for_best_nails_goes_to_by_opi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1fvs6yh</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Press-ons</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ac2q95fchosd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1fvs57b</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Happy Mean Girls Day💅🏻💋💄🎀</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvs57b</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1fvry3m</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>golden hour ✨️</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvry3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1fvrvn7</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>I’ve been obsessed with painting my own nails recently.</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dr9s19dcdosd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1fvr8o1</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>How to the get the intermediate colors on thermals?</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jndma9js5osd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1fvqhwx</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Best Ulta Haul So Far 💅🏼👌🏼✨</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10v576opxnsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1fvqffz</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Using 2 different top coat brand at same time </t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fvqffz/using_2_different_top_coat_brand_at_same_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1fvq77i</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Looking for a better way to pour acetone.</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fvq77i/looking_for_a_better_way_to_pour_acetone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1fvpj1d</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Twilight Sonata</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvpj1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1fvpcm7</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>PPU- Vintage Halloween</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4t3vgmqzlnsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1fvp6l9</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Riddle Me This </t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aauivl3bknsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1fvp1ol</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>First time stamping!</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvp1ol</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1fvoucn</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Subtle spooky</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvoucn</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1fvoe55</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to use cat eye polish and magnet? </t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fvoe55/how_to_use_cat_eye_polish_and_magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1fvo3yy</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Cosmic Polish Cassiopeia</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvo3yy</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1fvnon6</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I add thinner to my shimmers? </t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fvnon6/can_i_add_thinner_to_my_shimmers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1fvnc7u</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>"For the Twill of it" appreciation post</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bhvz353x2nsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1fvmw4c</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Zoya Envy turned my nails green</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fvmw4c/zoya_envy_turned_my_nails_green/</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1fvmtyk</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Let’s Rejoicify - OPIxWicked </t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8utua1b8ymsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1fvlq0d</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Sparkle. Shift. Sassy.</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bl7g0d3homsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1fvldgx</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>First galaxy nails attempt!</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvldgx</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1fvlch6</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Magnetic polish for days</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3t27ohw7lmsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1fvl9qx</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>First time using dotting tools</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wfa3yrkkkmsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1fvkr6i</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>September Mani Roundup</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvkr6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1fvk7we</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Cadillacquer | The Evil Dead (September PPU)</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvk7we</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1fvjwkx</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Brick and Mortar: while you’re in Minnesota to see Atomic’s store, check out some local nail supply stores</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fvjwkx/brick_and_mortar_while_youre_in_minnesota_to_see/</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1fvjup3</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Dupe for discontinued Formula X shade “Fine Like Einstein”?</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvjup3</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1fvjmhi</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail Art Round 2 </t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvjmhi</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1fvjl01</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Looking for a Dupe for Nicole by Opi's Sounds Grape to Me - It's not sold anymore and it's one of my favorite colors...</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvjl01</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1fvjk7e</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Is something going on with Chameleon Nails?</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fvjk7e/is_something_going_on_with_chameleon_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1fvjfhf</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Birthday Nails 🎉🥳💅🏼</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvjfhf</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1fvip2p</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Freebie prototype(?) shade I got with my Clionadh order: "Bloodline"</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/1cquDG6</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1fvi135</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Multi chrome, meet shorties 🤝</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dlhcoz24ulsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1fvh6vj</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>short smokey nails after big nail break</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvh6vj</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1fvgout</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Getting back into it!</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/78adkwryjlsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1fvgdlv</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Back with another Dollar General polish </t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvgdlv</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1fvfkn8</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jelly Polish + Glitter Ombré </t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdp8jnqablsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1fvfber</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>I trim my nails regularly. Don't clip the corners deep. What can I do about constant hangnails? Especially when I work with gloves.</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ahg8fe269lsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1fvf4km</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Ok LA Colors</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvf4km</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1fveopf</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Fierce Mojo 💜🩷⚡️</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6okv2bqn4lsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1fveh7a</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Need help finding this shade</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fveh7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1fvdcgv</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>goblins and ghoulies 👻💜</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvdcgv</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1fvd5d5</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Cheapest 30lb magnet?</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fvd5d5/cheapest_30lb_magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1fvd2f2</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Matching my nails to my ghost</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sczlrhddsksd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1fvceyo</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Please help me find a dupe! Gelixer #157</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvceyo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1fvcd9q</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why do essie nail polishes smell so bad? </t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fvcd9q/why_do_essie_nail_polishes_smell_so_bad/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1fvc143</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Top Coat Recs</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fvc143/top_coat_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1fvbmte</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Beautometry Question</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fvbmte/beautometry_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1fvbkf3</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do Cirque Wide Brushes fit Zoya bottles? </t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fvbkf3/do_cirque_wide_brushes_fit_zoya_bottles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1fvbcj6</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Slowly back to my old length! </t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvbcj6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1fvazbg</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Simply shreeeik</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvazbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1fvatqt</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Olive and June polish and hives?!</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fvatqt/olive_and_june_polish_and_hives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1fvacoa</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>🌈🦇Rainbow Bats🦇🌈</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvacoa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1fva4sv</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fva4sv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1fva30f</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone else having trouble with the PPU site? </t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fva30f/anyone_else_having_trouble_with_the_ppu_site/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1fv9pp9</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Matched my nails to my new dice set!</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v6lguhw82ksd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1fv8hnp</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>First try at magnetics</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fv8hnp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1fv817v</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Spooky Unicorn</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fv817v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1fv6mmk</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>please help find dupe - Polish Picture Forest</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1zgg4movcjsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1fv67az</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>This finish 🤤</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f56c909u8jsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1fv5wfi</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Monster Mash</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xfqdzwdt5jsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1fv5i7j</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my nails done for my wedding! </t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9pl25msq1jsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1fv53vx</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Advice on polish storage</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fv53vx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1fv4v0y</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Garden Path Lacquers - Always Dark </t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fv4v0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1fvtt8c</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is the best toolbox/suitcase for nail equipment? </t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fvtt8c/what_is_the_best_toolboxsuitcase_for_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1fvsm2e</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Spooky Skeleton Cat Nails 🐈‍⬛🦴</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4l8saonmosd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1fvslo9</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trick or Treat… Todays Halloween Special 👻 </t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2ce849vimosd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1fvrv58</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>HR Giger / Alien nails</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvrv58</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1fvqkpv</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Jujutsu Kaisen x Mochi Donuts!</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvqkpv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1fvq99l</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Butterfly wings 🦋</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvq99l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1fvpo4q</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Summer nails dump</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvpo4q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1fvorh7</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>My Sailor Moon Nails!</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/roxa4jlagnsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1fvm6qr</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Halloween nails</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/002az9bjsmsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1fvm578</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>💙💙</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvm578</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1fvkz7o</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>I made myself a metal press-on</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvkz7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1fvk6m1</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Pastel vibes</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ox4cmzb9bmsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1fvgj5v</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spoopy Season is here 🎃 </t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uwzwjaarilsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1fvehcz</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>3D Ghostface!</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/et85kuz33lsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1fve44u</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>3D Gel Fun</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1d29mnd0lsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1fvd8zn</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>My halloween "little ghosties" attempt really took a turn. 👻</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oybls9dptksd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1fvcash</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Just a wee bit wicked</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9k5a7qjmksd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1fvc5wn</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This Nails are very perfect by: vero di palazzio </t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvc5wn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1fvbknx</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>🎃🎃🎃</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uq751g72gksd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1fvbbyq</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ready for Halloween! </t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/alab7xwbeksd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1fvakel</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Full set hand painted on myself 🧡🖤💅🏼</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvakel</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1fva7b0</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Claw nails in Toronto/GTA</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fva7b0/claw_nails_in_torontogta/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1fva241</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Vampire nails inspired by Wolfinlace on insta</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fva241</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1fv86mm</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween Nails </t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1tbkfak3qjsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1fv80iv</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Another day of DIY &amp; learning~ </t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xqg4u8enojsd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1fv6hqq</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Experimenting and Seeing Where I Ended Up….</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1kk49wjnbjsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1fv6c8f</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>angel nails by me</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fv6c8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1fv2umy</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first attempt, how did I go? </t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3hjxf5703isd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Oct  5 08:09:16 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_06.xlsx
+++ b/data/collected_data/2024_10_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1047"/>
+  <dimension ref="A1:C1222"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18232,6 +18232,2981 @@
         </is>
       </c>
     </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1fwl0z7</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Should I text my nail tech if I'm not happy about 1 nail?</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xe5kagmm4wsd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1fwjrdq</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Fantasy blue ✨</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7eyzoa9ovsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1fwjob6</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail lady keeps on slaying </t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jsjbtjw6nvsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1fwhucw</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>EXTREMELY THIN NAILS</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fwhucw/extremely_thin_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1fwiysp</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>I love doing nails 🤩💅🏻</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwiysp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1fwh2ih</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Can anyone tell me why my polish NEVER dries???</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zlsolgb1uusd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1fwiom9</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Ombre claws!</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwiom9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1fwibm9</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red Black Gold / Lace set to kick start the halloween season! </t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwibm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1fwhxjz</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Advice on nail polish?</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwhxjz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1fwhri3</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Thermal nail polish , this is my absolute favourite.</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o5l1u2161vsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1fwhh4g</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checkers ♥ </t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00fat8o5yusd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1fwhcd6</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Emily de Molly - Enjoy the Fall 🍂🍁</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwhcd6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1fwhblu</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>leopard print frenchies🍒</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwhblu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1fwhauz</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bug nails ! </t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwhauz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1fwfo8g</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>help how do i fix this</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19s1u2q3gusd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1fwgxuh</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome butterflies </t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwgxuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1fwguw4</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>🐈‍⬛👻</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwguw4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1fwgbph</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>For those seamlessly transitioning into fall...</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iimne7ogmusd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1fwgaj5</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Got them done at Newme Nail Salon</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwgaj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1fwfsog</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Got my sparkly halloween nails🎃</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9f8rjixdhusd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1fwfmzh</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>👻</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwfmzh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1fwepoz</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Beetlejuice beetlejuice!</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1w1214zs6usd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1fweniy</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Frickin bats </t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wr61e3o86usd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1fwemg6</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matte Halloween set </t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0w2zg90z5usd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1fwegj5</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Spooky nails</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ylb8xvuf4usd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1fwe9rk</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I rid my nails and they look better in real life I promise </t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwe9rk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1fwe9ff</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spirited away🤩 cheap nails but I love them 🤩 </t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jd7pgx1n2usd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1fwe5x4</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>How to Fix?</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwe5x4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1fwe1wz</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>So obsessed with this Halloween set i got!</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfrpdmqr0usd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1fwe16l</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t xml:space="preserve">soft goth princess nails </t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxviyhvk0usd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1fwdyjr</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Squeaky clean! </t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwdyjr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1fwdxu5</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stars coz I’m a star </t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwdxu5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1fwaxb2</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Emergency! Please help, need nails for Monday and not sure what to ask for at appointment tomorrow. </t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18weczfo9tsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1fwcp9f</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>One month of growth!!! what design should I do now on my nails ?</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ti70ychmotsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1fwcns5</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My friend's Halloween manicure </t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwcns5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1fwcmj4</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Found my nail girl at last!</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwcmj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1fwca17</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Week 1 of Spooky Season</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwca17</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1fwc9y0</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried something new </t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwc9y0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1fwc9ru</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Berry on trend this season 🍇</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwc9ru</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1fwbret</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did some fun Halloween nails </t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/572xe8gkgtsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1fwb76l</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Spooky season begins👻🪦</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w8r7eq9xbtsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1fwb4wp</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>My girlfriend’s new nails, sorry for the bad quality photos for the last two</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwb4wp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1fwaz8g</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>🥰🥰😍</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cw38oso4atsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1fwaxwu</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>I love them too much</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m197ivet9tsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1fwauqx</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My birthday present from my amazing boyfriend! </t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwauqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1fwat49</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Worth a second complaint?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwat49</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1fwamte</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Lost my job this week for ridiculous reasons but at least my nails look ok</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/irdqt9nd7tsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1fwadn1</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Anyone else wonder?</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fwadn1/anyone_else_wonder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1fw9zx4</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Clean simple mani to let my new ring shine</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw9zx4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1fw9q85</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not even a minute later I almost lost my own nail </t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ms7gcj9b0tsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1fw9npg</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I haven't done my nails in years </t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw9npg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1fw8ae4</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Literally obsessed with my WITCHY BIRTHDAY NAILS 🧙🏾‍♀️🎃</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw8ae4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1fw9rho</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Halloween nails 🩸</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tvijhrtk0tsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1fw8xna</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>spooky nails</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1m4mqxp3ussd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1fw858c</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Silly question.</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fw858c/silly_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1fw7wx9</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Halloween nails🎃🎃🎃</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72tcshm4mssd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1fw7wcu</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail art newbie </t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw7wcu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1fw7n9z</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this because I pushed my cuticle back? </t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lscxdj61kssd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1fw7cbl</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Transitional Nails</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dwy1ufrohssd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1fw6xz1</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>🍂 ILNP Olive Grove with Painted Polish Gilded Olive 🫒</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw6xz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1fw6fu4</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This set makes me feel like the ultimate Baddie. </t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4navbwsassd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1fw6ce7</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">October vibes </t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cej8qdf2assd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1fw66ls</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>My wedding nails!</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/haosptsu8ssd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1fw63ge</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Gel-X to other Service?</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fw63ge/gelx_to_other_service/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1fw5ziw</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Natural nails ❀</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nnrn4nnc7ssd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1fw5y6d</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Encapsulated plants and bee wings (ethically sourced of course)</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw5y6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1fw5jfk</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>This is Halloween💚🕷️🖤🕸️</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw5jfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1fw4p0a</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Saw these on the sub and knew I had to make them🦋 Inspo from u/YeahTheyKnowItsMe</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw4p0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1fw4muk</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>🐇</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t30qood4xrsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1fw4eyv</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Y’all convinced me to go back to almond ….</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw4eyv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1fvxyry</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Time For Fall nails! </t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvxyry</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1fw3gp9</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail girl scared me with the fluorescent orange base coat, but I LOVE how these turned out. </t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8t6v6eccorsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1fw3cot</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Am I being silly or should I complain?</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw3cot</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1fw3bwg</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Update on my nail journey ☀️</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw3bwg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1fw1ak5</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Is there a reason why my nail tech would put nail glue under regular gel polish?</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fw1ak5/is_there_a_reason_why_my_nail_tech_would_put_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1fvu7ov</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Spooky season is on</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/91c69spi8psd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1fw37y4</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Simple Halloween nails</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9kl6a13jmrsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1fw34xi</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Natural nail flex</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xcwk0umwlrsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1fw2nyf</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail too short for acrylics ? </t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1u1fucpgirsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1fw29v1</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Gel Nails for vacation in Greece!</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gdru6jhfrsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1fw1snm</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Happy October 🖤</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw1snm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1fw1qxq</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Hexed by Stellar Gel</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t97ul5sgbrsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1fw1nh5</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Set </t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nhwtdkhtarsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1fw1lny</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Showing off this beautiful fall color</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5nitpwfarsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1fw160n</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>What do you all think? I do my own gel nails, I'm not a professional.</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/na5ywsr87rsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1fw0x5v</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Enamorada 😍</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw0x5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1fw0js5</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>I made these..</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/itipzdmj2rsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1fw0jkz</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">latest set </t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4gf7tci2rsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1fvzpqq</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>I've been painting my nails for about a year. This is the best theve ever looked. I never knew how much work and time nice nails take. And thanks to everyone how posts their beautiful nails I love seeing everyone's fun colors.</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgp6000wvqsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1fvze3l</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Halloween should be a year long holiday</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvze3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1fvz9i0</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Bridesmaid nails for bestie</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvz9i0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1fvz99g</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lil Halloween nails </t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/df6j7prasqsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1fvz8pz</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>2nd home nails</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvz8pz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1fvyqhs</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Little cuties @lash_nails_pinellas</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rzqldgwnqsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1fvyfjr</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Witchy cat eye!! 🔮</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pmf4webalqsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1fvxr7p</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Getting this at the moment 😌</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wl17paexeqsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1fvxp70</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Cute Halloween nails</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvxp70</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1fvxoc7</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Nail oil vs lotion</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fvxoc7/nail_oil_vs_lotion/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1fvxmcn</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween 🎃 nails 💅 🤪 </t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvxmcn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1fvx7ko</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>2nd time ever doing nail art! Ready for Halloween!</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvx7ko</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1fwk40n</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Halloween Skittle 🐦‍⬛🩸🎃🖤🥀🕷️</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwk40n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1fwk40d</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Happy October!</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwk40d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1fwjule</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>moody green creme ✨️</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwjule</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1fwi52c</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The bee's knees! </t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zw8d73ed5vsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1fwi337</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jewel Beetle </t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fsuomj7r4vsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1fwhqt7</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I matched my birb by mistake. </t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3vuqui01vsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1fwhffn</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Vibrant Scents Double Bond base coat - you need it. </t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fwhffn/vibrant_scents_double_bond_base_coat_you_need_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1fwhbdu</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Emily de Molly - Enjoy the Fall 🍂🍁</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwhbdu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1fwh9nx</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Can I get more than two days?</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fwh9nx/can_i_get_more_than_two_days/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1fwh82d</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Ethereal Lacquer Meow</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/13ly03jjvusd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1fwh13s</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Alchemy-Monster Mash</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwh13s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1fwewaj</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>hc static dupe?</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fwewaj/hc_static_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1fweox1</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Frickin bats </t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mmnogqal6usd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1fwdtm3</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Honestly shocked how fast the new Cirque Delusion collection got to me!</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mec5kq7jytsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1fwdnjc</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Olive and June sparkly nails</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwdnjc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1fwdgyi</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Arcana Lacquer!</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwdgyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1fwd4kd</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>🔮🧲😭</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwd4kd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1fwbyhj</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Candlelight 🕯️</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwbyhj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1fwb3le</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rose gold </t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwb3le</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1fwb1cn</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Dark mermaid vibes!</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lyltdccmatsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1fwavb1</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Peek-a-bOoOoO</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwavb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1fwa2la</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what do I do 😭 my DVN order came like this </t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwa2la</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1fw98yu</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>My mani accidentally matching my new keycaps set! 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9oj8pokwssd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1fw8gi1</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>My thoughts about this polish in a single word: Disappointing.</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2511iklbqssd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1fw8716</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Maple latte color for early fall!</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw8716</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1fw852m</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t xml:space="preserve">No photo can do Ghosts of Hecate justice </t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c3001w2rnssd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1fw84ix</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Zoya Adina for Halloween 🕷️ (+sonic unicorn skin)</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw84ix</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1fw7cmu</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Lisa Frank nails</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kao6zzcrhssd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1fw6yjj</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Completely obsessed with Haunted Vibes</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw6yjj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1fw6x81</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>🍂 ILNP Olive Grove with Painted Polish Gilded Olive 🫒</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw6x81</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1fw6avl</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t xml:space="preserve">October vibes </t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zvw2x6cr9ssd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1fw68n6</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Polish removal!</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fw68n6/polish_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1fw62v9</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>🍂🎃 A balmy 108° today to really get that fall vibe 🎃🍂</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw62v9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1fw5u30</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>What are some pale grayish lavender jelly or crelly polishes?</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lmswoph76ssd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1fw5cc4</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Is it okay to cry every time you use a polish that's discontinued 😭😭</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ymgsmzfj2ssd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1fw3rng</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>We don’t talk about Bunnies, Bunny! 🐇🥀</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw3rng</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1fw3dp6</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Wicked X OPI Ozitively Elphaba in direct sunlight</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw3dp6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1fw38q5</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cassiopeia by Cirque magnetized two ways </t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d7xticjpmrsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1fw2zek</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>€1 xoxo jelly dupe</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw2zek</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1fw2y9g</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Mooncat Bottles?</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fw2y9g/mooncat_bottles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1fw13sm</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Does anyone know of a sparkly blue that matches this shade? Been playing a lot of Elden ring and what to do my nails to match LOL</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8cx9rqjs6rsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1fw0w81</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Autumn leaves jellies! Psyche Minerals and LA Colors </t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw0w81</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1fw0v62</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>(Gifted PR/ad) ILNP Coven launches today!</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw0v62</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1fw03s0</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Arcana My Life as a Shrimp 🦐 🍤</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw03s0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1fvzcz5</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Phoenix Polish 🩵🩷</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0o64vf06tqsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1fvyvap</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bio sculpture(EVO gel) vs Dip powder </t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fvyvap/bio_sculptureevo_gel_vs_dip_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1fvybti</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Grave consequences 👻</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvybti</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1fvyaxp</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>What’s a ghost’s favourite type of pasta? Spook-ghetti 🍝</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvyaxp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1fvxt95</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Question about Seche Vite + a few other questions</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fvxt95/question_about_seche_vite_a_few_other_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1fvxo96</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help me pick the best sheer pinky for my pinkie. </t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/97g90vp5eqsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1fvx27h</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Finally got around to using QDTC and it's life changing. Not more bed sheet marks</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e77qfha38qsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1fvvdhh</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Is it okay to only put top coat (Glisten &amp; Glow) on your nails for protection against breakage when you don’t have time for a full mani?</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fvvdhh/is_it_okay_to_only_put_top_coat_glisten_glow_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1fvv5ez</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>How to open stubborn bottles without damaging nails/surfaces?</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fnu14nvflpsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1fvv3gz</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>exploring drugstore foils 🤩</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4x46xpfqkpsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1fwk3mf</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Scream Nails!</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwk3mf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1fwi51p</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lily of the Valley Ghosts </t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwi51p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1fwhyof</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Something I did today</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/klhzedbd3vsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1fwhohx</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>First time trying nail art! :-)</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwhohx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1fwhh5w</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Checkers ♥ </t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1umtqb6yusd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1fwgihf</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Have neuropathy and pain in my hands but I tried Halloween nails !!!💅 </t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwgihf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1fweo5k</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Courage The Cowardly Dog</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1n5bw52e6usd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1fwe9rt</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Freestyle set by Maya at bluebird nails (me :D)</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwe9rt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1fwcf4f</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Week 1 of Spooky Season</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwcf4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1fw9go5</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Can you tell what I was going for?</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw9go5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1fw8qjg</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Halloween nails🧡🖤🧡🖤💚</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/14po685jsssd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1fw8hb8</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love heart design tips </t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xdr73qpgqssd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1fw7aga</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A few of my favorite nail sets from the past </t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw7aga</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1fw6hz7</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Subtle Pastel Halloween </t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cmf6n63abssd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1fw5x30</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>🍁🍁🍁</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gkvto1zt6ssd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1fw5mfi</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Spring Nails</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jaeiq2xl4ssd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1fw5kal</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>hand painted sets</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw5kal</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1fw1nwy</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Set </t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ucj1oqwarsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1fvz9uu</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Halloween set! 🕸️</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvz9uu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1fvycqd</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween fun nails </t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fvycqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1fvv6ak</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Spooky Skeleton Cat Nails, designed and hand painted by Nikki Nailed it (I.e me!!) 🐈‍⬛🦴</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0sa6mw9slpsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Oct  6 08:09:18 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_06.xlsx
+++ b/data/collected_data/2024_10_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1222"/>
+  <dimension ref="A1:C1410"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21207,6 +21207,3202 @@
         </is>
       </c>
     </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1fxb8hw</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>You all loved the previous blinged set. Here’s another one but in ✨pink✨</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9zy9tr1ia3td1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1fxawa2</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Largest squares I've ever had</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4glu2a97x2td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1fxaq80</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>I love the touch of pink and glitter</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sqtnlhax33td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1fxalpj</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Anybody watch The Salon Life?</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fxalpj/anybody_watch_the_salon_life/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1fxa7vu</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>nails</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fxa7vu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1fwygn6</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>any ideas on how to make my nails stronger?</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwygn6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1fx8dyz</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>healthy nail journey, tips pls!</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx8dyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1fx900z</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Scary Nails 🩸🕷️🕸️👻</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx900z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1fx9ydm</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Went for a simple cat eye/magnet/velvet nail </t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hkewuyuyt2td1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1fx9yad</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Do you Like it?</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g16am90yt2td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1fx9wa0</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Gel overlay, what to buy?</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fx9wa0/gel_overlay_what_to_buy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1fx9iny</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t xml:space="preserve">"Fluorescent fuchsia that mesmerizes" </t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4j1k0nho2td1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1fx872l</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nails repair help </t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fx872l/nails_repair_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1fx735v</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>At Home Gel Nails Wipe Off</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fx735v/at_home_gel_nails_wipe_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1fwz0dh</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Is this a normal nail experience?</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwz0dh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1fx99na</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painted my fingernails for the first time (male) </t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx99na</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1fx948u</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press ons I did on myself </t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx948u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1fx92i7</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t xml:space="preserve">“The other salon damaged your nails!” </t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fx92i7/the_other_salon_damaged_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1fx91b7</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>bog witch/ decay/ grime nails</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx91b7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1fx8z1q</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Halloween set 1</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx8z1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1fx8xkl</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Yay! I finally did it!</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx8xkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1fx8u8l</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not too sure if I like my French tips </t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx8u8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1fx8pkm</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Horror movie nails</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx8pkm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1fx8lv7</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>DIY GEL NAILS</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fx8lv7/diy_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1fx8jci</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Should I take a break from doing my nails and let them recover, or are they not too bad?</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx8jci</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1fx87ky</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Fall colors for October</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i716q7f692td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1fx7w96</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fx7w96/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1fx7lxu</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Some DIY Goth glam...</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx7lxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1fx7a4v</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>New to press ons. Do they look okay?</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dezou7c3z1td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1fx6be1</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Real nails </t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/invgcy11p1td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1fx65kz</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Burgundy and pink with white and burgundy details </t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hc35appfn1td1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1fx5x7c</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recently did a Russian Manicure, and I don't think I can go back. </t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uuwpivt5l1td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1fx5ved</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Can these still be filled?</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1glaatgnk1td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1fx5l5g</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>It's not perfect but it's the first time I've done the french myself</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2oxh2r7ph1td1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1fx593z</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using gelx with aura trend </t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx593z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1fx56sc</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>🎃it's that time of the year</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx56sc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1fx40zy</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Press on help!?!</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fx40zy/press_on_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1fx3mtx</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Nail art improvement</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx3mtx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1fx3xqr</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>I’ve found my go-to nail lady 🥹</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx3xqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1fx55of</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>spooky szn (first post 💕)</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9q2o18bd1td1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1fx4zp9</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>First time making my own press-ons</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eynlhd2pb1td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1fx4gyt</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Very happy with my nails and they match with everything </t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gddca04p61td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1fx45oh</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Princess rule 🥰</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx45oh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1fx3kqt</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Halloween Nails!!!</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx3kqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1fx2owj</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Seche Vite dries gritty?</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fx2owj/seche_vite_dries_gritty/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1fwyqb1</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>LISA "New Woman" Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/panc7mweszsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1fx3ci5</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Beetlejuice</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3xga7j8w0td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1fx2yil</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my 5th set! </t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pvzd7pors0td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1fx2xks</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Showing I don't always walk around with dry af cuticles 😅</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0b1mi4js0td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1fx2qa6</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Witchy Cat Eye Nails 😍 </t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1basc9qq0td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1fx1hp3</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Halloween set</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/irajimymf0td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1fx1ckt</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>I would prefer if sparkles were flat, but I still pretty happy with this manicure! What do you think?</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5wwusefe0td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1fx189s</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>I'm so proud of doing it myself</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggq5pwsdd0td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1fx11fm</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>New October nails! First time doing an edgier look</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx11fm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1fx0ia7</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t xml:space="preserve">At home gel first time doing swirls. </t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uuk6ekh670td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1fx09p3</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing gel nails </t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oyekstd650td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1fx07p4</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>First long almonds I ever made</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fx07p4/first_long_almonds_i_ever_made/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1fwzn25</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Halloween glow nails</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n2mkfaiwzzsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1fwzku2</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I finally tried a new colour </t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7ng9jbezzsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1fwzdyb</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is your opinion on this almond-shaped nail design? </t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vrivsfrsxzsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1fwz02z</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>3 nails in and ambivalent about the color, opinions pls ☺️</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qpiao0eouzsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1fwyxrf</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Brown Sugar Icing Nails (admittedly a bit early in the year)</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bztoiqh1uzsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1fwytuh</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BEETLEJUICE BEETLEJUICE BEETLEJUICE </t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwytuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1fwyrmw</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>DIY Pastel Gradient (with bonus cat)</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/3EeKRLu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1fwy6ap</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Do press on nails cause damage?</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fwy6ap/do_press_on_nails_cause_damage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1fwy5sv</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Best method for French tips?</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fwy5sv/best_method_for_french_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1fwxuj2</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Opinions?</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwxuj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1fwxqdx</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Beetlejuice, Beetlejuice, Beetlejuice!</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/twj5as6fkzsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1fwxiwe</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Ombre nails…long nails are pretty too…who else love long nails 😍😍😍</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k56p5edrizsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1fwx9c1</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Autumn nails</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ndd72m2lgzsd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1fwx29u</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>My nail tech is AMAZING 🩷</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwx29u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1fwwy3l</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Attempting to summon cooler weather with my nails 😅</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwwy3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1fwu6r5</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Tequila!</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1aanr5itrysd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1fww4ko</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Shorter days, darker nails 🌚</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fww4ko</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1fww9ut</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Nails snap off- why!</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fww9ut</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1fww9bj</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Cute and spooky!</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k78483df8zsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1fww6v7</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>My thumbnails are half-black-half-white too, but it's not visible from.this angle. Thank you, mom, for taking the picture :)</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/svbbei8r7zsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1fwvy98</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love them </t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lpmnzicy5zsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1fwvwc1</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>College Game Day Nails</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwvwc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1fwvpqm</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Never tried purple </t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwvpqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1fwvoa0</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Love to do nude color on pedicure 💔 like or not?</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/385vzl8m3zsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1fwvkm8</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Halloween Nails + First time stamping</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1jm0tos2zsd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1fwv2f5</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Pearls,gems, charms it’s a good set as long as it’s 3d</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uxy6zhroyysd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1fwv0iu</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Jack nails!</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/odrtttkayysd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1fwuymo</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Gift ideas for someone new to dip manicures?</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fwuymo/gift_ideas_for_someone_new_to_dip_manicures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1fwuwa7</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>My Halloween nails 👻🎃</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r105i2qcxysd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1fwui86</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>My favorite set so far</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwui86</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1fwuhoo</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>are my press ons loose or do they just feel like that?</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0nq2h4s8uysd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1fwuhkj</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>What nail shape would you recommend for my hands? Long or short?</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7fj1a2p7uysd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1fwuc4r</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Soooo in love with this color </t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yauoll31tysd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1fwu4hp</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Butter London or Tweezerman GLASS nail file?</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fwu4hp/butter_london_or_tweezerman_glass_nail_file/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1fwty2l</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>My nails for this week. What do you think? I did it myself.</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xbzd6qpupysd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1fwttvn</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky 🕸️ 🎃 </t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwttvn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1fwt1kx</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>At home gel Strawberries!</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwt1kx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1fwsye1</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>A classic ❤️</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwsye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1fwsxex</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Is lacquer alone enough to hold these kinds of designs?</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9c85h53physd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1fwmzy2</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>My best discovery this year - water base nail polish</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwmzy2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1fwqwq9</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>How do you find new designs?</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fwqwq9/how_do_you_find_new_designs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1fwsi1s</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>How do I remove acrylic nails?</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1fwsi1s/how_do_i_remove_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1fwso2t</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Cherry red nails for fall 🍒🍁</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwso2t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1fx9ys1</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Screaming crying throwing up</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w1kaxct3u2td1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1fx9do5</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Making Nail Polish</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fx9do5/making_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1fx8x1z</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using magnetics and WOW! </t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx8x1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1fx7x2g</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Are all glow in the dark top coats like this?</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yryoyil062td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1fx7jrl</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>I know this one won't be for everyone...</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uud7xqhz12td1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1fx7a7b</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Gothic Cathedral Windows</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx7a7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1fx6xjb</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">holo nude is so magical </t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx6xjb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1fx6lhg</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Acrylate allergy</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fx6lhg/acrylate_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1fx642h</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Fair Isle and Crater Lake 🏞️</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx642h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1fx5aay</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Recreate with regular polish</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/DAtensCuWtk/?igsh=dWU4ZnRranlleGU3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1fx52ko</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>I’m hooked and I can’t stop staring 🎶</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx52ko</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1fx4xij</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Definitely deep in my fall phase</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx4xij</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1fx4cgz</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Feelin’ Capricorn-y</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx4cgz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1fx46co</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP High Voltage is so cute </t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ju6zw1vw31td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1fx3pct</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The hype is so real. </t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwlua4hgz0td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1fx3dy3</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When Your Nails are Classy but Your Shirt is Trashy </t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx3dy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1fx2zxu</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally, a Nail Polish that Matches my Personality—Monarch—Psycho </t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx2zxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1fx2tdb</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Cookies and Cream inspo nails 🍪🥛</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5wrz98iir0td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1fx2p6n</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Seche Vite dries gritty?</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fx2p6n/seche_vite_dries_gritty/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1fx2obc</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Bebio regular lacquer bio seeweed</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fx2obc/bebio_regular_lacquer_bio_seeweed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1fx2j48</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>New shade I just got. Love the green!</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u9v43q0yo0td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1fx2dnj</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Looking for some STORMY toned polishes.</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fx2dnj/looking_for_some_stormy_toned_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1fx2by3</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Is HB Beauty Bar legit?</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fx2by3/is_hb_beauty_bar_legit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1fx28pg</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First Halloween-ish nails! </t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx28pg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1fx1rfy</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A Light in the Storm </t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx1rfy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1fx1rdx</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>IYKYK</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx1rdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1fx1qj8</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Can't get enough of Halloween nails</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx1qj8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1fx1fkh</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>going through a red phase 🩸♥️</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx1fkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1fx19ew</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Insane drug store polish</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx19ew</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1fx0z8c</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Ethereal nail polish combo 💫😁</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx0z8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1fx0e14</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>First time getting gel nails, what all red flags should I look for?</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fx0e14/first_time_getting_gel_nails_what_all_red_flags/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1fx01vy</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Some Stamping Fun</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx01vy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1fwzvxp</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>First time ordering from ILNP</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9vebah020td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1fwzoze</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Costco Pepperoni Pizza</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7tnst7d00td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1fwzf5z</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painting over (and then removing polish from) shellac </t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fwzf5z/painting_over_and_then_removing_polish_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1fwzbjw</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Spooooooky Halloween!!!</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/olu7ts68xzsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1fwyyup</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Please help me find a dupe for this 15-year old polish from CVS!</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwyyup</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1fwy6iq</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do press on or glue on nails cause any damage to the natural nail? </t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fwy6iq/do_press_on_or_glue_on_nails_cause_any_damage_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1fwy42q</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>What is the best method for French tips?</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fwy42q/what_is_the_best_method_for_french_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1fwxzxm</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Looking for a creme pastel (almost neon) mint green polish with blue undertones</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fwxzxm/looking_for_a_creme_pastel_almost_neon_mint_green/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1fwxt2h</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Fall stamping</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwxt2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1fwx6f5</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Drugstore Creme Rainbow - REVIEW</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bao8mbfxfzsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1fwx4pd</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>I know Cirque Colors isn’t exactly at the top of everyone’s list right now… but</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0d3ln1gifzsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1fwx0la</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>We have red with an orange shimmer at home</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwx0la</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1fwwwz5</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>It's giving shiny pumpkin smoker nails but I'm into it.</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwwwz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1fwwpkk</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Autumn shimmer for an "Over The Garden Wall" party! </t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zqz7ufg2czsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1fwwmuo</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Attempting to summon fall weather with my mani 😅 (it's not working)</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwwmuo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1fwwjd3</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Nail art I did a couple of weeks back!</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwwjd3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1fwwir9</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>New to nail art</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uegywqdiazsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1fww7ui</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Essie Pillow Talk the talk</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fww7ui</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1fww3zo</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The first of many Halloween themed manis </t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40jxkbo77zsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1fww1vo</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky nails 🕸️ 🦇 </t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fww1vo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1fwvuu0</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Cal Bears Game Day Nails</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwvuu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1fwviiz</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking to get into making my own polish, where do I begin? </t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fwviiz/looking_to_get_into_making_my_own_polish_where_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1fwve4p</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Cellophane nails</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/huegikxa1zsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1fwvdnb</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Essie - Gilded Galaxy</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9f0nac671zsd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1fwv23w</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>🖤🩶Stark Silver🩶🖤</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwv23w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1fwubdv</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Now that spooky season is here, I thought I’d do some comparison swatches of ILNP’s black polishes. 🧙‍♀️</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwubdv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1fwttlw</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nightmare Before Christmas by yours truly </t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwttlw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1fwtmo2</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Orange nails for fall and spooky season 🎃👻</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwtmo2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1fwt2sr</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Happy James Bond Day! It took a few months of searching, but I have finally completed the OPI Skyfall collection!</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwt2sr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1fwrzzi</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Still managed to do a quick mani even with a 6 day old baby! </t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6iv5sp74aysd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1fwrgns</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Spooky nails to distract from the 100° forecast 🥵</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9ga3hdk5ysd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1fwq7nq</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Fancy Gloss Pearls as Toppers?</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fwq7nq/fancy_gloss_pearls_as_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1fwpxe3</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Does anyone know of a dupe for this discontinued glitter polish?</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zfo6lmsvrxsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1fwpoda</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>How do you know what nail shape suits you?</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fwpoda/how_do_you_know_what_nail_shape_suits_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1fwphqj</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Dream Within a Dream</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9z2wxqxtnxsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1fwotxz</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>A little 🌟glow🌟 for spooky season</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwotxz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1fwnx6u</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>The ultimate goth glitter polish!</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwnx6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1fwn4q2</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Are all Jellies Gel polish?</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fwn4q2/are_all_jellies_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1fw6cwr</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Short bitten nails blog</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://bittenswatches.blogspot.com/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1fwm440</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>What’s a good brand nail polish for a beginner?</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1fwm440/whats_a_good_brand_nail_polish_for_a_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1fw9fj4</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Marketplace find!</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fw9fj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1fxba51</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Usahana press on set</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ezoyndk9b3td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1fxb32g</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>Gradient/ombre w/ gel polish?</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8e7h9e2j83td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1fx923b</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>bog witch/ decay/ grime nails</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx923b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1fx77fe</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Cateye press-ons with some celestial art</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx77fe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1fx6fuu</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Batty for these nails! </t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10f0x5v9q1td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1fx578o</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t xml:space="preserve">me regalan su opinión del color? </t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wuhe31x6d1td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1fx4v86</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>I’m so proud of these 🖤</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fx4v86</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1fx2vhh</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>90’s Nail Designs</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1fx2vhh/90s_nail_designs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1fx0r64</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Gel X Nails made by myself (collage)</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2haibw1a90td1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1fwz4wz</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Season of the Witch</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2y0cggkrvzsd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1fwwx7o</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Did some fall nails in an attempt to summon cooler weather 😅</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwwx7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1fwug9l</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>2nd time doing my own acrylics, 1st time using blooming gel 😬</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwug9l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1fws93l</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>First attempt at Halloween nails</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fws93l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1fwqze4</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My mom’s first time using builder gel- I’m sure excited to be wearing these!! 🥰 </t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2fh9qke1ysd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1fwqder</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Pretty Scary Part Trois</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1fwqder</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>